<commit_message>
Die Einträge vom Lernjournal aus dem 1. Semester für die Aufagabe 3 ins neue Übetragen
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="440" windowWidth="29720" windowHeight="18940" tabRatio="415"/>
+    <workbookView xWindow="17700" yWindow="1140" windowWidth="29720" windowHeight="18940" tabRatio="415"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -87,6 +87,33 @@
   <si>
     <t>Organisation der Ablage und Abtrennen der 3. Aufgabe aus dem letzen Dokument.
 Alles Vorbereitet für neues Semester.</t>
+  </si>
+  <si>
+    <t>Fachklassendiagramm ( Aufgabe 1 ) erstellt - 1 Version - Vorschlag</t>
+  </si>
+  <si>
+    <t>Glossar ( Aufgabe 4 ) Vorschlag</t>
+  </si>
+  <si>
+    <t>Besprechung Gruppe</t>
+  </si>
+  <si>
+    <t>Fachklassendiagramm ( Aufgabe 1 ) erstellt - 2 und 3 Version - Vorschlag</t>
+  </si>
+  <si>
+    <t>Fachklassendiagramm zusammengeführt - Vereinheitlicht, Versucht richtige Lösung für das Glosser zu finden. Begriffe nach unserem Verständniss der Aufgabenstellung definiert und beschreiben.</t>
+  </si>
+  <si>
+    <t>Dokument angepasst. Neue Aufgabenstellunge eingebaut und Lyout angepasst.</t>
+  </si>
+  <si>
+    <t>Korrekturen erster Teil, soweit möglich, eingearbeit.</t>
+  </si>
+  <si>
+    <t>Fachklassendiagramm erstellt (inkl. Besprechung bei der Arbeit über das Wie?)!</t>
+  </si>
+  <si>
+    <t>Anwendungsfall Diagramm angepasst - neue Version / Ideen</t>
   </si>
 </sst>
 </file>
@@ -209,8 +236,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -376,14 +419,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="89">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -420,6 +463,14 @@
     <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -456,6 +507,14 @@
     <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -785,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -818,11 +877,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -993,15 +1052,15 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="24">
+    <row r="11" spans="1:16" s="11" customFormat="1">
       <c r="A11" s="27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="28">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C11" s="29">
-        <v>41535</v>
+        <v>41434</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -1018,9 +1077,15 @@
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" s="11" customFormat="1">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
+      <c r="A12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="28">
+        <v>5</v>
+      </c>
+      <c r="C12" s="29">
+        <v>41434</v>
+      </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1036,9 +1101,15 @@
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:16" s="11" customFormat="1">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
+      <c r="A13" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="28">
+        <v>45</v>
+      </c>
+      <c r="C13" s="29">
+        <v>41434</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1054,9 +1125,15 @@
       <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="27"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="25">
+        <v>30</v>
+      </c>
+      <c r="C14" s="26">
+        <v>41436</v>
+      </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1071,10 +1148,16 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A15" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="25">
+        <v>105</v>
+      </c>
+      <c r="C15" s="26">
+        <v>41441</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1091,8 +1174,8 @@
     </row>
     <row r="16" spans="1:16" s="11" customFormat="1">
       <c r="A16" s="27"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1108,9 +1191,9 @@
       <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -1125,10 +1208,10 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="12"/>
+    <row r="18" spans="1:16" s="11" customFormat="1">
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1143,72 +1226,72 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:16" s="4" customFormat="1">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:16" s="11" customFormat="1">
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" s="11" customFormat="1">
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="1:16" s="4" customFormat="1">
+      <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="18">
-        <f>SUM(B11:B18)</f>
-        <v>35</v>
-      </c>
-      <c r="C19" s="19">
-        <f>TIME(0,B19,)</f>
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" s="4" customFormat="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" s="4" customFormat="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" s="4" customFormat="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="18">
+        <f>SUM(B11:B21)</f>
+        <v>230</v>
+      </c>
+      <c r="C22" s="19">
+        <f>TIME(0,B22,)</f>
+        <v>0.15972222222222224</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1223,14 +1306,10 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A23" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="23" spans="1:16" s="4" customFormat="1">
+      <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1264,15 +1343,9 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" s="4" customFormat="1">
-      <c r="A25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1287,64 +1360,80 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1">
-      <c r="A26" s="25"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-    </row>
-    <row r="27" spans="1:16" s="11" customFormat="1">
-      <c r="A27" s="25"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-    </row>
-    <row r="28" spans="1:16" s="11" customFormat="1">
-      <c r="A28" s="25"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
+    <row r="26" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" s="4" customFormat="1">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" s="4" customFormat="1">
+      <c r="A28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" s="11" customFormat="1">
-      <c r="A29" s="25"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="30"/>
+      <c r="A29" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="23">
+        <v>20</v>
+      </c>
+      <c r="C29" s="24">
+        <v>41433</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1360,9 +1449,15 @@
       <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16" s="11" customFormat="1">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="31"/>
+      <c r="A30" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="28">
+        <v>25</v>
+      </c>
+      <c r="C30" s="29">
+        <v>41434</v>
+      </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1378,9 +1473,15 @@
       <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:16" s="11" customFormat="1">
-      <c r="A31" s="25"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="30"/>
+      <c r="A31" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="28">
+        <v>50</v>
+      </c>
+      <c r="C31" s="29">
+        <v>41440</v>
+      </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1396,9 +1497,15 @@
       <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:16" s="11" customFormat="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
+      <c r="A32" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="28">
+        <v>15</v>
+      </c>
+      <c r="C32" s="29">
+        <v>41439</v>
+      </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -1413,10 +1520,16 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" s="11" customFormat="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
+    <row r="33" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A33" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="25">
+        <v>105</v>
+      </c>
+      <c r="C33" s="26">
+        <v>41441</v>
+      </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -1431,10 +1544,16 @@
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="12"/>
+    <row r="34" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A34" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="28">
+        <v>35</v>
+      </c>
+      <c r="C34" s="29">
+        <v>41535</v>
+      </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -1449,112 +1568,108 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" s="4" customFormat="1">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:16" s="11" customFormat="1">
+      <c r="A35" s="27"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" s="11" customFormat="1">
+      <c r="A36" s="27"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" s="11" customFormat="1">
+      <c r="A37" s="20"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+    </row>
+    <row r="38" spans="1:16" s="11" customFormat="1">
+      <c r="A38" s="20"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" s="4" customFormat="1">
+      <c r="A40" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="18">
-        <f>SUM(B26:B34)</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="19">
-        <f>TIME(0,B35,)</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-    </row>
-    <row r="36" spans="1:16" s="4" customFormat="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-    </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
-      <c r="A39" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-    </row>
-    <row r="40" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="18">
+        <f>SUM(B29:B39)</f>
+        <v>250</v>
+      </c>
+      <c r="C40" s="19">
+        <f>TIME(0,B40,)</f>
+        <v>0.17361111111111113</v>
+      </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1569,16 +1684,10 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>6</v>
-      </c>
+    <row r="41" spans="1:16" s="4" customFormat="1">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1593,80 +1702,67 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A42" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="8">
-        <v>0</v>
-      </c>
-      <c r="C42" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-    </row>
-    <row r="43" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="8">
-        <v>0</v>
-      </c>
-      <c r="C43" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-    </row>
-    <row r="44" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
+    <row r="42" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+    </row>
+    <row r="43" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A45" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="14">
-        <f>SUM(B42:B44)</f>
-        <v>0</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="3"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1682,31 +1778,144 @@
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
     </row>
-    <row r="47" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
-      <c r="A47" s="15" t="s">
+    <row r="46" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A46" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+    </row>
+    <row r="47" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A47" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="8">
+        <v>0</v>
+      </c>
+      <c r="C47" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+    </row>
+    <row r="48" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="8">
+        <v>0</v>
+      </c>
+      <c r="C48" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+    </row>
+    <row r="49" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+    </row>
+    <row r="50" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A50" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="14">
+        <f>SUM(B47:B49)</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+    </row>
+    <row r="52" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A52" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="16">
-        <f>SUM(B35,B19)</f>
-        <v>35</v>
-      </c>
-      <c r="C47" s="17">
-        <f>TIME(0,B47,)</f>
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
+      <c r="B52" s="16">
+        <f>SUM(B40,B22)</f>
+        <v>480</v>
+      </c>
+      <c r="C52" s="17">
+        <f>TIME(0,B52,)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1764,11 +1973,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2668,11 +2877,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>

</xml_diff>

<commit_message>
Inhalte der Telefonkonferenz und TeamViewer Session zusammengestellt im Hauptdokument. Temporäre Daten aus Versionierung wieder entfernt
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17700" yWindow="1140" windowWidth="29720" windowHeight="18940" tabRatio="415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26860" windowHeight="18140" tabRatio="415"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -115,6 +115,18 @@
   <si>
     <t>Anwendungsfall Diagramm angepasst - neue Version / Ideen</t>
   </si>
+  <si>
+    <t>Fachklassendiagramm Aufgabe 3 Überarbeitet</t>
+  </si>
+  <si>
+    <t>Sequenzdiagramm erstellt</t>
+  </si>
+  <si>
+    <t>Fachklassen Glossar erstellt</t>
+  </si>
+  <si>
+    <t>Dokumente zusammengeführt</t>
+  </si>
 </sst>
 </file>
 
@@ -175,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -235,8 +247,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -326,8 +366,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -419,14 +467,41 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="97">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -471,6 +546,10 @@
     <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -515,6 +594,10 @@
     <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -844,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="A40" sqref="A40:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -877,11 +960,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1148,14 +1231,14 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="36">
-      <c r="A15" s="27" t="s">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
+      <c r="A15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="33">
         <v>105</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="34">
         <v>41441</v>
       </c>
       <c r="D15" s="10"/>
@@ -1172,10 +1255,16 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+      <c r="A16" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="36">
+        <v>35</v>
+      </c>
+      <c r="C16" s="37">
+        <v>41538</v>
+      </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1191,9 +1280,15 @@
       <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
+      <c r="A17" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="28">
+        <v>65</v>
+      </c>
+      <c r="C17" s="29">
+        <v>41538</v>
+      </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -1209,9 +1304,15 @@
       <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
+      <c r="A18" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="28">
+        <v>20</v>
+      </c>
+      <c r="C18" s="29">
+        <v>41538</v>
+      </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1262,10 +1363,10 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="12"/>
+    <row r="21" spans="1:16" s="11" customFormat="1">
+      <c r="A21" s="27"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1280,54 +1381,54 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:16" s="11" customFormat="1">
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+    </row>
+    <row r="23" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+    </row>
+    <row r="24" spans="1:16" s="4" customFormat="1">
+      <c r="A24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="18">
-        <f>SUM(B11:B21)</f>
-        <v>230</v>
-      </c>
-      <c r="C22" s="19">
-        <f>TIME(0,B22,)</f>
-        <v>0.15972222222222224</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="1:16" s="4" customFormat="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="1:16" s="4" customFormat="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
+      <c r="B24" s="18">
+        <f>SUM(B11:B23)</f>
+        <v>350</v>
+      </c>
+      <c r="C24" s="19">
+        <f>TIME(0,B24,)</f>
+        <v>0.24305555555555555</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1360,14 +1461,10 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A26" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="26" spans="1:16" s="4" customFormat="1">
+      <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1400,15 +1497,13 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" s="4" customFormat="1">
-      <c r="A28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>6</v>
+    <row r="28" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1424,63 +1519,57 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1">
-      <c r="A29" s="32" t="s">
+    <row r="29" spans="1:16" s="4" customFormat="1">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" s="4" customFormat="1">
+      <c r="A30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" s="11" customFormat="1">
+      <c r="A31" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B31" s="23">
         <v>20</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C31" s="24">
         <v>41433</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-    </row>
-    <row r="30" spans="1:16" s="11" customFormat="1">
-      <c r="A30" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="28">
-        <v>25</v>
-      </c>
-      <c r="C30" s="29">
-        <v>41434</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-    </row>
-    <row r="31" spans="1:16" s="11" customFormat="1">
-      <c r="A31" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="28">
-        <v>50</v>
-      </c>
-      <c r="C31" s="29">
-        <v>41440</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -1498,13 +1587,13 @@
     </row>
     <row r="32" spans="1:16" s="11" customFormat="1">
       <c r="A32" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B32" s="28">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C32" s="29">
-        <v>41439</v>
+        <v>41434</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1520,15 +1609,15 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" s="11" customFormat="1" ht="36">
-      <c r="A33" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="25">
-        <v>105</v>
-      </c>
-      <c r="C33" s="26">
-        <v>41441</v>
+    <row r="33" spans="1:16" s="11" customFormat="1">
+      <c r="A33" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="28">
+        <v>50</v>
+      </c>
+      <c r="C33" s="29">
+        <v>41440</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -1544,15 +1633,15 @@
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="1:16" s="11" customFormat="1" ht="24">
-      <c r="A34" s="27" t="s">
-        <v>14</v>
+    <row r="34" spans="1:16" s="11" customFormat="1">
+      <c r="A34" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="B34" s="28">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C34" s="29">
-        <v>41535</v>
+        <v>41439</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -1568,10 +1657,16 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" s="11" customFormat="1">
-      <c r="A35" s="27"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
+    <row r="35" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
+      <c r="A35" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="33">
+        <v>105</v>
+      </c>
+      <c r="C35" s="34">
+        <v>41441</v>
+      </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -1586,10 +1681,16 @@
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" spans="1:16" s="11" customFormat="1">
-      <c r="A36" s="27"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
+    <row r="36" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
+      <c r="A36" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="36">
+        <v>35</v>
+      </c>
+      <c r="C36" s="37">
+        <v>41535</v>
+      </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -1605,9 +1706,15 @@
       <c r="P36" s="10"/>
     </row>
     <row r="37" spans="1:16" s="11" customFormat="1">
-      <c r="A37" s="20"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
+      <c r="A37" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="28">
+        <v>35</v>
+      </c>
+      <c r="C37" s="29">
+        <v>41538</v>
+      </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -1623,9 +1730,15 @@
       <c r="P37" s="10"/>
     </row>
     <row r="38" spans="1:16" s="11" customFormat="1">
-      <c r="A38" s="20"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="28">
+        <v>65</v>
+      </c>
+      <c r="C38" s="29">
+        <v>41538</v>
+      </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -1640,10 +1753,16 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="12"/>
+    <row r="39" spans="1:16" s="11" customFormat="1">
+      <c r="A39" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="28">
+        <v>20</v>
+      </c>
+      <c r="C39" s="29">
+        <v>41538</v>
+      </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -1658,112 +1777,114 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:16" s="11" customFormat="1">
+      <c r="A40" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="28">
+        <v>15</v>
+      </c>
+      <c r="C40" s="30">
+        <v>41538</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" s="11" customFormat="1">
+      <c r="A41" s="38"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" s="11" customFormat="1">
+      <c r="A42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" s="4" customFormat="1">
+      <c r="A45" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="18">
-        <f>SUM(B29:B39)</f>
-        <v>250</v>
-      </c>
-      <c r="C40" s="19">
-        <f>TIME(0,B40,)</f>
-        <v>0.17361111111111113</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-    </row>
-    <row r="41" spans="1:16" s="4" customFormat="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-    </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-    </row>
-    <row r="43" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-    </row>
-    <row r="44" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
-      <c r="A44" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-    </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="3"/>
+      <c r="B45" s="18">
+        <f>SUM(B31:B44)</f>
+        <v>385</v>
+      </c>
+      <c r="C45" s="19">
+        <f>TIME(0,B45,)</f>
+        <v>0.2673611111111111</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -1778,16 +1899,10 @@
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A46" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>6</v>
-      </c>
+    <row r="46" spans="1:16" s="4" customFormat="1">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="3"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -1802,80 +1917,67 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A47" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="8">
-        <v>0</v>
-      </c>
-      <c r="C47" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-    </row>
-    <row r="48" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A48" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="8">
-        <v>0</v>
-      </c>
-      <c r="C48" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-    </row>
-    <row r="49" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
+    <row r="47" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A49" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
     </row>
     <row r="50" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A50" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="14">
-        <f>SUM(B47:B49)</f>
-        <v>0</v>
-      </c>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
       <c r="C50" s="3"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1891,31 +1993,144 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="52" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
-      <c r="A52" s="15" t="s">
+    <row r="51" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+    </row>
+    <row r="52" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A52" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="8">
+        <v>0</v>
+      </c>
+      <c r="C52" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+    </row>
+    <row r="53" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="8">
+        <v>0</v>
+      </c>
+      <c r="C53" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+    </row>
+    <row r="54" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+    </row>
+    <row r="55" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A55" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="14">
+        <f>SUM(B52:B54)</f>
+        <v>0</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+    </row>
+    <row r="57" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A57" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="16">
-        <f>SUM(B40,B22)</f>
-        <v>480</v>
-      </c>
-      <c r="C52" s="17">
-        <f>TIME(0,B52,)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
+      <c r="B57" s="16">
+        <f>SUM(B45,B24)</f>
+        <v>735</v>
+      </c>
+      <c r="C57" s="17">
+        <f>TIME(0,B57,)</f>
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1973,11 +2188,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2877,11 +3092,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>

</xml_diff>

<commit_message>
Aufgabe 3, Auftrag 3 Teil 1,2 und 4 soweit fertig gestellt
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -126,6 +126,10 @@
   </si>
   <si>
     <t>Dokumente zusammengeführt</t>
+  </si>
+  <si>
+    <t>Diagramme überarbeitet und Glossar verfeinert.
+Abgabefertig für's erste.</t>
   </si>
 </sst>
 </file>
@@ -276,8 +280,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -501,7 +507,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="99">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -550,6 +556,7 @@
     <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -598,6 +605,7 @@
     <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1327,10 +1335,16 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:16" s="11" customFormat="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
+    <row r="19" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="28">
+        <v>45</v>
+      </c>
+      <c r="C19" s="29">
+        <v>41545</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -1423,11 +1437,11 @@
       </c>
       <c r="B24" s="18">
         <f>SUM(B11:B23)</f>
-        <v>350</v>
+        <v>395</v>
       </c>
       <c r="C24" s="19">
         <f>TIME(0,B24,)</f>
-        <v>0.24305555555555555</v>
+        <v>0.27430555555555552</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1801,10 +1815,16 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" s="11" customFormat="1">
-      <c r="A41" s="38"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="40"/>
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A41" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="28">
+        <v>45</v>
+      </c>
+      <c r="C41" s="29">
+        <v>41545</v>
+      </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -1879,11 +1899,11 @@
       </c>
       <c r="B45" s="18">
         <f>SUM(B31:B44)</f>
-        <v>385</v>
+        <v>430</v>
       </c>
       <c r="C45" s="19">
         <f>TIME(0,B45,)</f>
-        <v>0.2673611111111111</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2112,11 +2132,11 @@
       </c>
       <c r="B57" s="16">
         <f>SUM(B45,B24)</f>
-        <v>735</v>
+        <v>825</v>
       </c>
       <c r="C57" s="17">
         <f>TIME(0,B57,)</f>
-        <v>0.51041666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>

</xml_diff>

<commit_message>
State-Diagramm edited and in other documents integrated. Lernjournal updated
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3_team_3_lernjournal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -131,6 +131,15 @@
     <t>Diagramme überarbeitet und Glossar verfeinert.
 Abgabefertig für's erste.</t>
   </si>
+  <si>
+    <t>Zustandsdiagram erste Entwurf erstellt</t>
+  </si>
+  <si>
+    <t>Diagramm besprochen und fertig gestellt</t>
+  </si>
+  <si>
+    <t>Dokumente ergeänzt und für Abgabe vorbereitet.</t>
+  </si>
 </sst>
 </file>
 
@@ -191,7 +200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -279,8 +288,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -380,8 +417,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -494,20 +533,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="101">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -557,6 +605,7 @@
     <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -606,6 +655,7 @@
     <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -937,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -968,11 +1018,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1335,14 +1385,14 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:16" s="11" customFormat="1" ht="24">
-      <c r="A19" s="27" t="s">
+    <row r="19" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
+      <c r="A19" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="40">
         <v>45</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="41">
         <v>41545</v>
       </c>
       <c r="D19" s="10"/>
@@ -1359,10 +1409,16 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="1:16" s="11" customFormat="1">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
+    <row r="20" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+      <c r="A20" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="43">
+        <v>30</v>
+      </c>
+      <c r="C20" s="44">
+        <v>41552</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1378,9 +1434,15 @@
       <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16" s="11" customFormat="1">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="28">
+        <v>60</v>
+      </c>
+      <c r="C21" s="29">
+        <v>41553</v>
+      </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1437,11 +1499,11 @@
       </c>
       <c r="B24" s="18">
         <f>SUM(B11:B23)</f>
-        <v>395</v>
+        <v>485</v>
       </c>
       <c r="C24" s="19">
         <f>TIME(0,B24,)</f>
-        <v>0.27430555555555552</v>
+        <v>0.33680555555555558</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1815,14 +1877,14 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" ht="24">
-      <c r="A41" s="27" t="s">
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
+      <c r="A41" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="28">
+      <c r="B41" s="40">
         <v>45</v>
       </c>
-      <c r="C41" s="29">
+      <c r="C41" s="41">
         <v>41545</v>
       </c>
       <c r="D41" s="10"/>
@@ -1839,10 +1901,16 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" s="11" customFormat="1">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40"/>
+    <row r="42" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+      <c r="A42" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="28">
+        <v>60</v>
+      </c>
+      <c r="C42" s="29">
+        <v>41553</v>
+      </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -1858,9 +1926,15 @@
       <c r="P42" s="10"/>
     </row>
     <row r="43" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="12"/>
+      <c r="A43" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="10">
+        <v>20</v>
+      </c>
+      <c r="C43" s="12">
+        <v>41553</v>
+      </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -1899,11 +1973,11 @@
       </c>
       <c r="B45" s="18">
         <f>SUM(B31:B44)</f>
-        <v>430</v>
+        <v>510</v>
       </c>
       <c r="C45" s="19">
         <f>TIME(0,B45,)</f>
-        <v>0.2986111111111111</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2132,11 +2206,11 @@
       </c>
       <c r="B57" s="16">
         <f>SUM(B45,B24)</f>
-        <v>825</v>
+        <v>995</v>
       </c>
       <c r="C57" s="17">
         <f>TIME(0,B57,)</f>
-        <v>0.57291666666666663</v>
+        <v>0.69097222222222221</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2208,11 +2282,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3112,11 +3186,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>

</xml_diff>